<commit_message>
update TestSuite Analysis Report
</commit_message>
<xml_diff>
--- a/TestSuite-Analysis/X509 Testsuite Analysis.xlsx
+++ b/TestSuite-Analysis/X509 Testsuite Analysis.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="75">
   <si>
     <t xml:space="preserve">Family</t>
   </si>
@@ -227,10 +227,34 @@
     <t xml:space="preserve">DuplicateCertificateTests</t>
   </si>
   <si>
+    <t xml:space="preserve">Root and Entity error - org.opentest4j.AssertionFailedError:  Expected :false Actual   :true // Intermediate error - java.lang.IllegalArgumentException: The expression must not evaluate to false</t>
+  </si>
+  <si>
     <t xml:space="preserve">SelfSignedNonRootTests</t>
   </si>
   <si>
+    <t xml:space="preserve">Entity error – ts.selfSignedEntity(SelfSignedNonRootTests.java:28) // Intermediate error - java.lang.IllegalArgumentException: The expression must not evaluate to false // Test in general failed with error – java.lang.AssertionError</t>
+  </si>
+  <si>
     <t xml:space="preserve">Version1IntermediateCertTests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Failed with error - java.lang.IllegalArgumentException: The expression must not evaluate to false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PositiveTests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UntrustedRootTests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BerInsteadOfDerTests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvalidCertificateLengthTests</t>
   </si>
 </sst>
 </file>
@@ -469,13 +493,13 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="73.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="179.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="9.14"/>
@@ -934,10 +958,16 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.58203125" defaultRowHeight="67.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="36.59375" defaultRowHeight="67.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="124.81"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -954,27 +984,45 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>64</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -993,13 +1041,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.29296875" defaultRowHeight="64.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="36.30078125" defaultRowHeight="64.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="144.65"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1015,6 +1069,32 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="72.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="80.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1031,15 +1111,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="37.15234375" defaultRowHeight="64.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="37.1640625" defaultRowHeight="66.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="137.48"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1051,6 +1137,16 @@
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1075,7 +1171,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.0078125" defaultRowHeight="67.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="36.015625" defaultRowHeight="67.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1113,7 +1209,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.29296875" defaultRowHeight="63.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="36.30078125" defaultRowHeight="63.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1151,7 +1247,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.8671875" defaultRowHeight="62.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="36.875" defaultRowHeight="62.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1189,7 +1285,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.72265625" defaultRowHeight="64.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="36.73046875" defaultRowHeight="64.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1227,7 +1323,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.29296875" defaultRowHeight="68.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="36.30078125" defaultRowHeight="68.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="68.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">

</xml_diff>